<commit_message>
start dealing with error
</commit_message>
<xml_diff>
--- a/LL parser/parsing table.xlsx
+++ b/LL parser/parsing table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B644D750-9A9B-458C-9483-F6AFCDAA9FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF529B22-433A-46CF-ABF3-C8A25B5BC51D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
   <si>
     <t>program</t>
   </si>
@@ -238,6 +238,14 @@
   </si>
   <si>
     <t>&gt;=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compoundstmt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,7 +575,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -651,6 +659,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -753,6 +764,9 @@
       <c r="H12" t="s">
         <v>47</v>
       </c>
+      <c r="N12" t="s">
+        <v>64</v>
+      </c>
       <c r="Q12" t="s">
         <v>47</v>
       </c>
@@ -774,6 +788,9 @@
       </c>
       <c r="H14" t="s">
         <v>47</v>
+      </c>
+      <c r="N14" t="s">
+        <v>64</v>
       </c>
       <c r="Q14" t="s">
         <v>47</v>

</xml_diff>